<commit_message>
Cleanup and small ui message improvements.
</commit_message>
<xml_diff>
--- a/cardinal-health-data-tracking.xlsx
+++ b/cardinal-health-data-tracking.xlsx
@@ -67,7 +67,7 @@
     <t xml:space="preserve">Estimated Hours</t>
   </si>
   <si>
-    <t xml:space="preserve">Assignment groupx</t>
+    <t xml:space="preserve">Assignment group</t>
   </si>
   <si>
     <t xml:space="preserve">[inc] 2:1</t>
@@ -8334,8 +8334,8 @@
   </sheetPr>
   <dimension ref="A1:M500"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M2" activeCellId="0" sqref="M2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>